<commit_message>
[Fix] Medical Column Name in Active List Reading From Excel
</commit_message>
<xml_diff>
--- a/src/MedicalMembersListTemplate-Empty.xlsx
+++ b/src/MedicalMembersListTemplate-Empty.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9215"/>
+    <workbookView windowWidth="28800" windowHeight="12375"/>
   </bookViews>
   <sheets>
     <sheet name="Medical List" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
-    <t>Id-Iqama No.</t>
+    <t>Id\Iqama No.</t>
   </si>
   <si>
     <t>Membership No</t>
@@ -72,9 +72,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="178" formatCode="m/d/yyyy;@"/>
   </numFmts>
@@ -97,6 +97,42 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -106,46 +142,41 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -165,29 +196,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -197,21 +205,36 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -220,29 +243,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -263,37 +263,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -305,19 +425,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -329,121 +437,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -472,11 +472,43 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -523,197 +555,165 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1089,27 +1089,27 @@
   <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2" outlineLevelRow="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelRow="3"/>
   <cols>
-    <col min="1" max="1" width="14.1388888888889" style="2" customWidth="1"/>
+    <col min="1" max="1" width="14.1428571428571" style="2" customWidth="1"/>
     <col min="2" max="2" width="18" style="2" customWidth="1"/>
-    <col min="3" max="3" width="16.287037037037" style="2" customWidth="1"/>
-    <col min="4" max="4" width="20.2592592592593" style="3" customWidth="1"/>
-    <col min="5" max="6" width="15.287037037037" style="2" customWidth="1"/>
-    <col min="7" max="7" width="8.71296296296296" style="2" customWidth="1"/>
-    <col min="8" max="8" width="13.287037037037" style="2" customWidth="1"/>
-    <col min="9" max="9" width="9.28703703703704" style="2" customWidth="1"/>
-    <col min="10" max="10" width="16.1388888888889" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16.2857142857143" style="2" customWidth="1"/>
+    <col min="4" max="4" width="20.2571428571429" style="3" customWidth="1"/>
+    <col min="5" max="6" width="15.2857142857143" style="2" customWidth="1"/>
+    <col min="7" max="7" width="8.71428571428571" style="2" customWidth="1"/>
+    <col min="8" max="8" width="13.2857142857143" style="2" customWidth="1"/>
+    <col min="9" max="9" width="9.28571428571429" style="2" customWidth="1"/>
+    <col min="10" max="10" width="16.1428571428571" style="2" customWidth="1"/>
     <col min="11" max="11" width="7" style="2" customWidth="1"/>
-    <col min="12" max="12" width="5.13888888888889" style="2" customWidth="1"/>
-    <col min="13" max="13" width="9.42592592592593" style="2" customWidth="1"/>
-    <col min="14" max="14" width="10.287037037037" style="2" customWidth="1"/>
-    <col min="15" max="15" width="11.4259259259259" style="2" customWidth="1"/>
-    <col min="16" max="16" width="11.8518518518519" style="2" customWidth="1"/>
-    <col min="17" max="17" width="13.8518518518519" style="2" customWidth="1"/>
+    <col min="12" max="12" width="5.14285714285714" style="2" customWidth="1"/>
+    <col min="13" max="13" width="9.42857142857143" style="2" customWidth="1"/>
+    <col min="14" max="14" width="10.2857142857143" style="2" customWidth="1"/>
+    <col min="15" max="15" width="11.4285714285714" style="2" customWidth="1"/>
+    <col min="16" max="16" width="11.847619047619" style="2" customWidth="1"/>
+    <col min="17" max="17" width="13.847619047619" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="15" spans="1:17">
@@ -1165,7 +1165,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" ht="13.8" spans="1:17">
+    <row r="2" ht="14.25" spans="1:17">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -1184,7 +1184,7 @@
       <c r="P2" s="6"/>
       <c r="Q2" s="6"/>
     </row>
-    <row r="3" ht="13.8" spans="1:17">
+    <row r="3" ht="14.25" spans="1:17">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -1203,7 +1203,7 @@
       <c r="P3" s="6"/>
       <c r="Q3" s="6"/>
     </row>
-    <row r="4" ht="13.8" spans="1:17">
+    <row r="4" ht="14.25" spans="1:17">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>

</xml_diff>